<commit_message>
Working on CUDA version, Parallel CPU version is working
</commit_message>
<xml_diff>
--- a/GPU DSGE Tools/Ex1_Serial.xlsx
+++ b/GPU DSGE Tools/Ex1_Serial.xlsx
@@ -457,25 +457,25 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>1.28975103456725</v>
+        <v>1.289713969429163</v>
       </c>
       <c r="C2">
-        <v>1.0405772204333</v>
+        <v>1.040549717476848</v>
       </c>
       <c r="D2">
-        <v>0.249173814133948</v>
+        <v>0.2491642519523148</v>
       </c>
       <c r="E2">
-        <v>0.196859699141985</v>
+        <v>0.1968626860971182</v>
       </c>
       <c r="F2">
-        <v>0.864133193160054</v>
+        <v>0.8641083595175394</v>
       </c>
       <c r="G2">
-        <v>2.16203645329929</v>
+        <v>2.161941513401254</v>
       </c>
       <c r="H2">
-        <v>3.7426742336256e-06</v>
+        <v>-1.752153088167524e-05</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -483,25 +483,25 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>0.000160882807567234</v>
+        <v>0.0001617203364274568</v>
       </c>
       <c r="C3">
-        <v>0.000109126642450099</v>
+        <v>0.0001095081546554957</v>
       </c>
       <c r="D3">
-        <v>5.53162007231447e-05</v>
+        <v>5.587731278983738e-05</v>
       </c>
       <c r="E3">
-        <v>1.62848460112334e-05</v>
+        <v>1.637100151948144e-05</v>
       </c>
       <c r="F3">
-        <v>0.000107791481070046</v>
+        <v>0.0001083526254063959</v>
       </c>
       <c r="G3">
-        <v>0.000337781407058016</v>
+        <v>0.0003378014666888245</v>
       </c>
       <c r="H3">
-        <v>0.000127150711838131</v>
+        <v>0.0001285032358530241</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -512,22 +512,22 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>0.674804664906672</v>
+        <v>0.6756238030766768</v>
       </c>
       <c r="D4">
-        <v>0.348052724294144</v>
+        <v>0.3474293626494357</v>
       </c>
       <c r="E4">
-        <v>0.103117812021036</v>
+        <v>0.1021510693381799</v>
       </c>
       <c r="F4">
-        <v>0.669999999999992</v>
+        <v>0.669999999999999</v>
       </c>
       <c r="G4">
-        <v>2.07693634999456</v>
+        <v>2.07943393139117</v>
       </c>
       <c r="H4">
-        <v>0.800874428181403</v>
+        <v>0.7993801889009886</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -538,22 +538,22 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>0.988359191941354</v>
+        <v>0.9884494485792923</v>
       </c>
       <c r="D5">
-        <v>0.956939684754782</v>
+        <v>0.9561650976675447</v>
       </c>
       <c r="E5">
-        <v>-0.0809176878453925</v>
+        <v>-0.07549240067504825</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="G5">
-        <v>0.834889427423557</v>
+        <v>0.8412700963316098</v>
       </c>
       <c r="H5">
-        <v>0.949504924919388</v>
+        <v>0.9485925684281818</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -561,25 +561,25 @@
         <v>11</v>
       </c>
       <c r="B6">
-        <v>0.946890772673335</v>
+        <v>0.9495053716747701</v>
       </c>
       <c r="C6">
-        <v>0.968455026821135</v>
+        <v>0.9705347381981705</v>
       </c>
       <c r="D6">
-        <v>0.895622045856594</v>
+        <v>0.8982627044924651</v>
       </c>
       <c r="E6">
-        <v>0.863964558163452</v>
+        <v>0.8649238768848985</v>
       </c>
       <c r="F6">
-        <v>0.94689077267334</v>
+        <v>0.9495053716747688</v>
       </c>
       <c r="G6">
-        <v>0.99169266943278</v>
+        <v>0.9922147479707973</v>
       </c>
       <c r="H6">
-        <v>0.891137701319112</v>
+        <v>0.8937818712849989</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -587,25 +587,25 @@
         <v>12</v>
       </c>
       <c r="B7">
-        <v>0.000124738956571942</v>
+        <v>0.0001253922401745724</v>
       </c>
       <c r="C7">
-        <v>0.000104870830123666</v>
+        <v>0.0001052405553871066</v>
       </c>
       <c r="D7">
-        <v>0.000221997840393045</v>
+        <v>0.0002242584882890124</v>
       </c>
       <c r="E7">
-        <v>8.27231448508433e-05</v>
+        <v>8.315952163916979e-05</v>
       </c>
       <c r="F7">
-        <v>0.00012473895657194</v>
+        <v>0.0001253922401745723</v>
       </c>
       <c r="G7">
-        <v>0.000156231797353881</v>
+        <v>0.0001562488713588043</v>
       </c>
       <c r="H7">
-        <v>-0.477536327626393</v>
+        <v>-11.20102049865351</v>
       </c>
     </row>
   </sheetData>
@@ -631,7 +631,7 @@
         <v>13</v>
       </c>
       <c r="B2">
-        <v>4.34909867708967e-05</v>
+        <v>4.34972889381401e-05</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -639,7 +639,7 @@
         <v>14</v>
       </c>
       <c r="B3">
-        <v>4.33656862581694e-05</v>
+        <v>4.333066796271318e-05</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -647,7 +647,7 @@
         <v>15</v>
       </c>
       <c r="B4">
-        <v>4.33705476578236e-05</v>
+        <v>4.333870639554767e-05</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -655,7 +655,7 @@
         <v>16</v>
       </c>
       <c r="B5">
-        <v>0.820229758212008</v>
+        <v>7.585690812714347</v>
       </c>
     </row>
   </sheetData>

</xml_diff>